<commit_message>
Update project files, add new column to xlsx-file
</commit_message>
<xml_diff>
--- a/file_example_XLSX_10.xlsx
+++ b/file_example_XLSX_10.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="40">
   <si>
     <t xml:space="preserve">Record Number</t>
   </si>
@@ -46,6 +46,9 @@
     <t xml:space="preserve">Id</t>
   </si>
   <si>
+    <t xml:space="preserve">Size</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dulce</t>
   </si>
   <si>
@@ -61,6 +64,9 @@
     <t xml:space="preserve">15/10/2017</t>
   </si>
   <si>
+    <t xml:space="preserve">L</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mara</t>
   </si>
   <si>
@@ -73,6 +79,9 @@
     <t xml:space="preserve">16/08/2016</t>
   </si>
   <si>
+    <t xml:space="preserve">M</t>
+  </si>
+  <si>
     <t xml:space="preserve">Philip</t>
   </si>
   <si>
@@ -88,12 +97,18 @@
     <t xml:space="preserve">21/05/2015</t>
   </si>
   <si>
+    <t xml:space="preserve">XL</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kathleen</t>
   </si>
   <si>
     <t xml:space="preserve">Hanner</t>
   </si>
   <si>
+    <t xml:space="preserve">S</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nereida</t>
   </si>
   <si>
@@ -110,6 +125,9 @@
   </si>
   <si>
     <t xml:space="preserve">Hurn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XS</t>
   </si>
   <si>
     <t xml:space="preserve">Earlean</t>
@@ -242,10 +260,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -278,31 +296,37 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>32</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H2" s="1" t="n">
         <v>1562</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -310,25 +334,28 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F3" s="1" t="n">
         <v>25</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H3" s="1" t="n">
         <v>1582</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -336,25 +363,28 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F4" s="1" t="n">
         <v>36</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H4" s="1" t="n">
         <v>2587</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -362,25 +392,28 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F5" s="1" t="n">
         <v>25</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H5" s="1" t="n">
         <v>3549</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -388,25 +421,28 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F6" s="1" t="n">
         <v>58</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H6" s="1" t="n">
         <v>2468</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -414,25 +450,28 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F7" s="1" t="n">
         <v>24</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H7" s="1" t="n">
         <v>2554</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -440,25 +479,28 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F8" s="1" t="n">
         <v>56</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H8" s="1" t="n">
         <v>3598</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -466,25 +508,28 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F9" s="1" t="n">
         <v>27</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H9" s="1" t="n">
         <v>2456</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -492,25 +537,28 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F10" s="1" t="n">
         <v>40</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H10" s="1" t="n">
         <v>6548</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>